<commit_message>
Put in some sample runs. Last three are on BAT. need to change the Bm- OH on other ones
</commit_message>
<xml_diff>
--- a/input_BAT2030.xlsx
+++ b/input_BAT2030.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C026B7FF-6AE6-4A91-BCED-4B229E15413A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F2A6C5AB-404F-49CF-9413-FA9623A36102}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -5455,7 +5455,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15876,8 +15876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15935,10 +15935,10 @@
         <v>1E-4</v>
       </c>
       <c r="G2" s="16">
-        <v>250</v>
+        <v>600</v>
       </c>
       <c r="H2" s="16">
-        <v>150</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -15951,7 +15951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1 more sample run
</commit_message>
<xml_diff>
--- a/input_BAT2030.xlsx
+++ b/input_BAT2030.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F2A6C5AB-404F-49CF-9413-FA9623A36102}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="288" windowWidth="14808" windowHeight="7836" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sources" sheetId="1" r:id="rId1"/>
@@ -17,17 +16,17 @@
     <sheet name="Restrictions" sheetId="6" r:id="rId7"/>
     <sheet name="EnergyTypes" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,12 +105,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +135,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -166,12 +165,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -196,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -251,12 +250,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="A1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -285,12 +284,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{2E592D98-4030-4E90-8CB3-408C9D0C4087}">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3055,7 +3054,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -3257,35 +3256,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:S167" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:S167" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:S167" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:S167"/>
   <sortState ref="A2:R167">
     <sortCondition ref="E1:E167"/>
   </sortState>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="FacilityID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="FacilityName"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="PostalCode"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="City"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Spalte2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TotalQuantity"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="[Mt CO2/a]">
+    <tableColumn id="1" name="FacilityID"/>
+    <tableColumn id="2" name="FacilityName"/>
+    <tableColumn id="3" name="PostalCode"/>
+    <tableColumn id="4" name="City"/>
+    <tableColumn id="5" name="Spalte2"/>
+    <tableColumn id="6" name="TotalQuantity"/>
+    <tableColumn id="7" name="[Mt CO2/a]">
       <calculatedColumnFormula>F2/10^9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Plant size [MW]" dataDxfId="0">
+    <tableColumn id="8" name="Plant size [MW]" dataDxfId="0">
       <calculatedColumnFormula>(G2/3.88*34.2*10^9)/(8000*3600)*0.9</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="MethodTypeName"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Spalte1"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="StreetName"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="BuildingNumber"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Lat"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Long"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="MainIAActivityCode"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="MainIASectorName"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="MainIAActivityName"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="MainIASubActivityName"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="CO2 Cost pkg"/>
+    <tableColumn id="9" name="MethodTypeName"/>
+    <tableColumn id="10" name="Spalte1"/>
+    <tableColumn id="11" name="StreetName"/>
+    <tableColumn id="12" name="BuildingNumber"/>
+    <tableColumn id="13" name="Lat"/>
+    <tableColumn id="14" name="Long"/>
+    <tableColumn id="15" name="MainIAActivityCode"/>
+    <tableColumn id="16" name="MainIASectorName"/>
+    <tableColumn id="17" name="MainIAActivityName"/>
+    <tableColumn id="18" name="MainIASubActivityName"/>
+    <tableColumn id="19" name="CO2 Cost pkg"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3334,7 +3333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3367,26 +3366,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3419,23 +3401,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3611,22 +3576,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -3811,20 +3776,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -3995,43 +3960,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="7" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" style="15" customWidth="1"/>
     <col min="10" max="10" width="5" style="7" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="9.44140625" customWidth="1"/>
-    <col min="18" max="18" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="9.42578125" customWidth="1"/>
+    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -4096,7 +4061,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
@@ -4157,7 +4122,7 @@
         <v>0.13978494623655915</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>832</v>
       </c>
@@ -4214,7 +4179,7 @@
       <c r="T3" s="16"/>
       <c r="U3" s="16"/>
     </row>
-    <row r="4" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="8" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>860</v>
       </c>
@@ -4268,7 +4233,7 @@
       <c r="U4" s="16"/>
       <c r="V4" s="9"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>31</v>
       </c>
@@ -4321,7 +4286,7 @@
       <c r="T5" s="16"/>
       <c r="U5" s="16"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>30</v>
       </c>
@@ -4374,7 +4339,7 @@
       <c r="T6" s="16"/>
       <c r="U6" s="16"/>
     </row>
-    <row r="7" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="10" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>862</v>
       </c>
@@ -4427,7 +4392,7 @@
       <c r="T7" s="16"/>
       <c r="U7" s="16"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>891</v>
       </c>
@@ -4480,7 +4445,7 @@
       <c r="T8" s="16"/>
       <c r="U8" s="16"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>892</v>
       </c>
@@ -4533,7 +4498,7 @@
       <c r="T9" s="16"/>
       <c r="U9" s="16"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>11</v>
       </c>
@@ -4590,7 +4555,7 @@
       <c r="T10" s="16"/>
       <c r="U10" s="16"/>
     </row>
-    <row r="11" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="11" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>833</v>
       </c>
@@ -4653,7 +4618,7 @@
       <c r="V11" s="12"/>
       <c r="X11" s="12"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>834</v>
       </c>
@@ -4718,7 +4683,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>863</v>
       </c>
@@ -4775,7 +4740,7 @@
       <c r="T13" s="16"/>
       <c r="U13" s="16"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>893</v>
       </c>
@@ -4832,7 +4797,7 @@
       <c r="T14" s="16"/>
       <c r="U14" s="16"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>894</v>
       </c>
@@ -4889,7 +4854,7 @@
       <c r="T15" s="16"/>
       <c r="U15" s="16"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>50</v>
       </c>
@@ -4942,7 +4907,7 @@
       <c r="T16" s="16"/>
       <c r="U16" s="16"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>51</v>
       </c>
@@ -4995,7 +4960,7 @@
       <c r="T17" s="16"/>
       <c r="U17" s="16"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>44</v>
       </c>
@@ -5048,7 +5013,7 @@
       <c r="T18" s="16"/>
       <c r="U18" s="16"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>45</v>
       </c>
@@ -5101,7 +5066,7 @@
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>58</v>
       </c>
@@ -5150,7 +5115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>59</v>
       </c>
@@ -5199,7 +5164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>864</v>
       </c>
@@ -5248,7 +5213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>865</v>
       </c>
@@ -5297,7 +5262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>866</v>
       </c>
@@ -5346,7 +5311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>867</v>
       </c>
@@ -5395,7 +5360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>868</v>
       </c>
@@ -5451,21 +5416,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5479,7 +5444,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>835</v>
       </c>
@@ -5493,7 +5458,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>836</v>
       </c>
@@ -5507,7 +5472,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>869</v>
       </c>
@@ -5521,7 +5486,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>32</v>
       </c>
@@ -5535,7 +5500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -5549,7 +5514,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>870</v>
       </c>
@@ -5563,7 +5528,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="16" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>895</v>
       </c>
@@ -5577,7 +5542,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="16" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>896</v>
       </c>
@@ -5591,7 +5556,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>34</v>
       </c>
@@ -5605,7 +5570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>837</v>
       </c>
@@ -5619,7 +5584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>838</v>
       </c>
@@ -5633,7 +5598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>871</v>
       </c>
@@ -5647,7 +5612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" s="16" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>897</v>
       </c>
@@ -5661,7 +5626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" s="16" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>904</v>
       </c>
@@ -5675,7 +5640,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>839</v>
       </c>
@@ -5689,7 +5654,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>840</v>
       </c>
@@ -5703,7 +5668,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>841</v>
       </c>
@@ -5717,7 +5682,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="15" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>886</v>
       </c>
@@ -5731,7 +5696,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" s="16" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>898</v>
       </c>
@@ -5745,7 +5710,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" s="16" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>899</v>
       </c>
@@ -5759,7 +5724,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>842</v>
       </c>
@@ -5773,7 +5738,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="14" t="s">
         <v>843</v>
       </c>
@@ -5787,7 +5752,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>844</v>
       </c>
@@ -5801,7 +5766,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>846</v>
       </c>
@@ -5815,7 +5780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>847</v>
       </c>
@@ -5829,7 +5794,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>872</v>
       </c>
@@ -5843,7 +5808,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>37</v>
       </c>
@@ -5857,7 +5822,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>38</v>
       </c>
@@ -5871,7 +5836,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>874</v>
       </c>
@@ -5885,7 +5850,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>900</v>
       </c>
@@ -5899,7 +5864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>901</v>
       </c>
@@ -5913,7 +5878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>39</v>
       </c>
@@ -5927,7 +5892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>848</v>
       </c>
@@ -5941,7 +5906,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>849</v>
       </c>
@@ -5955,7 +5920,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>850</v>
       </c>
@@ -5969,7 +5934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>851</v>
       </c>
@@ -5983,7 +5948,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>852</v>
       </c>
@@ -5997,7 +5962,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>875</v>
       </c>
@@ -6011,7 +5976,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>902</v>
       </c>
@@ -6025,7 +5990,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>903</v>
       </c>
@@ -6039,7 +6004,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>40</v>
       </c>
@@ -6053,7 +6018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>52</v>
       </c>
@@ -6067,7 +6032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>876</v>
       </c>
@@ -6081,7 +6046,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>46</v>
       </c>
@@ -6095,7 +6060,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>47</v>
       </c>
@@ -6109,7 +6074,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>60</v>
       </c>
@@ -6123,7 +6088,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>61</v>
       </c>
@@ -6137,7 +6102,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>877</v>
       </c>
@@ -6151,7 +6116,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>878</v>
       </c>
@@ -6165,7 +6130,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>879</v>
       </c>
@@ -6179,7 +6144,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>880</v>
       </c>
@@ -6193,7 +6158,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>853</v>
       </c>
@@ -6207,7 +6172,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>41</v>
       </c>
@@ -6221,7 +6186,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>53</v>
       </c>
@@ -6235,7 +6200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>881</v>
       </c>
@@ -6249,7 +6214,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>48</v>
       </c>
@@ -6263,7 +6228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>49</v>
       </c>
@@ -6277,7 +6242,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>62</v>
       </c>
@@ -6291,7 +6256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>63</v>
       </c>
@@ -6305,7 +6270,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>882</v>
       </c>
@@ -6319,7 +6284,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>883</v>
       </c>
@@ -6333,7 +6298,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>884</v>
       </c>
@@ -6347,7 +6312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>885</v>
       </c>
@@ -6367,14 +6332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -6482,35 +6447,35 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S167"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
     <col min="9" max="9" width="46" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
     <col min="13" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.88671875" customWidth="1"/>
-    <col min="16" max="16" width="20.44140625" customWidth="1"/>
-    <col min="17" max="17" width="21.5546875" customWidth="1"/>
-    <col min="18" max="18" width="24.88671875" customWidth="1"/>
+    <col min="15" max="15" width="20.85546875" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" customWidth="1"/>
+    <col min="18" max="18" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -6569,7 +6534,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>43104</v>
       </c>
@@ -6627,7 +6592,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>43106</v>
       </c>
@@ -6685,7 +6650,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>43123</v>
       </c>
@@ -6743,7 +6708,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>43110</v>
       </c>
@@ -6798,7 +6763,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>70297</v>
       </c>
@@ -6856,7 +6821,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>43127</v>
       </c>
@@ -6914,7 +6879,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>43581</v>
       </c>
@@ -6969,7 +6934,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>43561</v>
       </c>
@@ -7027,7 +6992,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>43735</v>
       </c>
@@ -7082,7 +7047,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>43366</v>
       </c>
@@ -7137,7 +7102,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>104967</v>
       </c>
@@ -7192,7 +7157,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>43246</v>
       </c>
@@ -7247,7 +7212,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>73883</v>
       </c>
@@ -7305,7 +7270,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43203</v>
       </c>
@@ -7360,7 +7325,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>54392</v>
       </c>
@@ -7415,7 +7380,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>220711</v>
       </c>
@@ -7473,7 +7438,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>43243</v>
       </c>
@@ -7528,7 +7493,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>43205</v>
       </c>
@@ -7586,7 +7551,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>73896</v>
       </c>
@@ -7644,7 +7609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>43348</v>
       </c>
@@ -7702,7 +7667,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>69944</v>
       </c>
@@ -7757,7 +7722,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>105004</v>
       </c>
@@ -7812,7 +7777,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>104958</v>
       </c>
@@ -7867,7 +7832,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>43721</v>
       </c>
@@ -7922,7 +7887,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>73960</v>
       </c>
@@ -7980,7 +7945,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>110171</v>
       </c>
@@ -8035,7 +8000,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>70343</v>
       </c>
@@ -8090,7 +8055,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>43505</v>
       </c>
@@ -8148,7 +8113,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>43407</v>
       </c>
@@ -8203,7 +8168,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>43614</v>
       </c>
@@ -8258,7 +8223,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>43611</v>
       </c>
@@ -8313,7 +8278,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>44489</v>
       </c>
@@ -8368,7 +8333,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>44251</v>
       </c>
@@ -8426,7 +8391,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>44252</v>
       </c>
@@ -8484,7 +8449,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>43600</v>
       </c>
@@ -8539,7 +8504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>110145</v>
       </c>
@@ -8594,7 +8559,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>43597</v>
       </c>
@@ -8649,7 +8614,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>43484</v>
       </c>
@@ -8707,7 +8672,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>43306</v>
       </c>
@@ -8762,7 +8727,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>43428</v>
       </c>
@@ -8820,7 +8785,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>43455</v>
       </c>
@@ -8875,7 +8840,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>43283</v>
       </c>
@@ -8930,7 +8895,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43479</v>
       </c>
@@ -8985,7 +8950,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44389</v>
       </c>
@@ -9043,7 +9008,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44419</v>
       </c>
@@ -9098,7 +9063,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>44435</v>
       </c>
@@ -9153,7 +9118,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>43257</v>
       </c>
@@ -9208,7 +9173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>43298</v>
       </c>
@@ -9266,7 +9231,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>46977</v>
       </c>
@@ -9321,7 +9286,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>46915</v>
       </c>
@@ -9379,7 +9344,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>74832</v>
       </c>
@@ -9434,7 +9399,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>46986</v>
       </c>
@@ -9489,7 +9454,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>46849</v>
       </c>
@@ -9544,7 +9509,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>46947</v>
       </c>
@@ -9602,7 +9567,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>44668</v>
       </c>
@@ -9660,7 +9625,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>44705</v>
       </c>
@@ -9715,7 +9680,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>110415</v>
       </c>
@@ -9770,7 +9735,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>110279</v>
       </c>
@@ -9825,7 +9790,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>44684</v>
       </c>
@@ -9880,7 +9845,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>47048</v>
       </c>
@@ -9938,7 +9903,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>44670</v>
       </c>
@@ -9993,7 +9958,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>44746</v>
       </c>
@@ -10051,7 +10016,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>43815</v>
       </c>
@@ -10106,7 +10071,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>43860</v>
       </c>
@@ -10164,7 +10129,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>71068</v>
       </c>
@@ -10219,7 +10184,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>44323</v>
       </c>
@@ -10277,7 +10242,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>74041</v>
       </c>
@@ -10332,7 +10297,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>44246</v>
       </c>
@@ -10387,7 +10352,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>44302</v>
       </c>
@@ -10442,7 +10407,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>43884</v>
       </c>
@@ -10497,7 +10462,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>43942</v>
       </c>
@@ -10552,7 +10517,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>157889</v>
       </c>
@@ -10607,7 +10572,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>43870</v>
       </c>
@@ -10665,7 +10630,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>43872</v>
       </c>
@@ -10720,7 +10685,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>43938</v>
       </c>
@@ -10775,7 +10740,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>43818</v>
       </c>
@@ -10830,7 +10795,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>43941</v>
       </c>
@@ -10885,7 +10850,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>43822</v>
       </c>
@@ -10940,7 +10905,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>43820</v>
       </c>
@@ -10995,7 +10960,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>43819</v>
       </c>
@@ -11050,7 +11015,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>43917</v>
       </c>
@@ -11108,7 +11073,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>43779</v>
       </c>
@@ -11163,7 +11128,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>43935</v>
       </c>
@@ -11218,7 +11183,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>43895</v>
       </c>
@@ -11273,7 +11238,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>43934</v>
       </c>
@@ -11328,7 +11293,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>43847</v>
       </c>
@@ -11383,7 +11348,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>43971</v>
       </c>
@@ -11441,7 +11406,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>46236</v>
       </c>
@@ -11496,7 +11461,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>43878</v>
       </c>
@@ -11551,7 +11516,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>43784</v>
       </c>
@@ -11609,7 +11574,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>43804</v>
       </c>
@@ -11667,7 +11632,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>44199</v>
       </c>
@@ -11722,7 +11687,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>43913</v>
       </c>
@@ -11780,7 +11745,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>43794</v>
       </c>
@@ -11835,7 +11800,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>43842</v>
       </c>
@@ -11893,7 +11858,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>44733</v>
       </c>
@@ -11951,7 +11916,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>44799</v>
       </c>
@@ -12006,7 +11971,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>44820</v>
       </c>
@@ -12061,7 +12026,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>46317</v>
       </c>
@@ -12119,7 +12084,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>110413</v>
       </c>
@@ -12174,7 +12139,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>46322</v>
       </c>
@@ -12232,7 +12197,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>46378</v>
       </c>
@@ -12287,7 +12252,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>74742</v>
       </c>
@@ -12345,7 +12310,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>74758</v>
       </c>
@@ -12400,7 +12365,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>46982</v>
       </c>
@@ -12455,7 +12420,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>73639</v>
       </c>
@@ -12510,7 +12475,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>74855</v>
       </c>
@@ -12568,7 +12533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>46914</v>
       </c>
@@ -12623,7 +12588,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>110066</v>
       </c>
@@ -12681,7 +12646,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>46834</v>
       </c>
@@ -12739,7 +12704,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>46837</v>
       </c>
@@ -12794,7 +12759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>46949</v>
       </c>
@@ -12852,7 +12817,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>46830</v>
       </c>
@@ -12907,7 +12872,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>46897</v>
       </c>
@@ -12965,7 +12930,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>46944</v>
       </c>
@@ -13020,7 +12985,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>46956</v>
       </c>
@@ -13078,7 +13043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>46955</v>
       </c>
@@ -13136,7 +13101,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>46869</v>
       </c>
@@ -13191,7 +13156,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>46945</v>
       </c>
@@ -13246,7 +13211,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>44053</v>
       </c>
@@ -13301,7 +13266,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>44485</v>
       </c>
@@ -13356,7 +13321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>44486</v>
       </c>
@@ -13411,7 +13376,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>44484</v>
       </c>
@@ -13466,7 +13431,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>110204</v>
       </c>
@@ -13521,7 +13486,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>74009</v>
       </c>
@@ -13576,7 +13541,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>44061</v>
       </c>
@@ -13631,7 +13596,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>44090</v>
       </c>
@@ -13686,7 +13651,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>44142</v>
       </c>
@@ -13741,7 +13706,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>74015</v>
       </c>
@@ -13796,7 +13761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>44060</v>
       </c>
@@ -13851,7 +13816,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>200990</v>
       </c>
@@ -13909,7 +13874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>110205</v>
       </c>
@@ -13964,7 +13929,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>44138</v>
       </c>
@@ -14022,7 +13987,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>44098</v>
       </c>
@@ -14077,7 +14042,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>44067</v>
       </c>
@@ -14132,7 +14097,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>70868</v>
       </c>
@@ -14187,7 +14152,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>44162</v>
       </c>
@@ -14242,7 +14207,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>44123</v>
       </c>
@@ -14297,7 +14262,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>44128</v>
       </c>
@@ -14355,7 +14320,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>74350</v>
       </c>
@@ -14410,7 +14375,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>57513</v>
       </c>
@@ -14465,7 +14430,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>44882</v>
       </c>
@@ -14520,7 +14485,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>45027</v>
       </c>
@@ -14575,7 +14540,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>45034</v>
       </c>
@@ -14633,7 +14598,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>189271</v>
       </c>
@@ -14688,7 +14653,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>71806</v>
       </c>
@@ -14743,7 +14708,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>71805</v>
       </c>
@@ -14798,7 +14763,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>73702</v>
       </c>
@@ -14853,7 +14818,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>46988</v>
       </c>
@@ -14911,7 +14876,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>46989</v>
       </c>
@@ -14969,7 +14934,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>46987</v>
       </c>
@@ -15027,7 +14992,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>56260</v>
       </c>
@@ -15082,7 +15047,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>45063</v>
       </c>
@@ -15140,7 +15105,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>44037</v>
       </c>
@@ -15195,7 +15160,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>110284</v>
       </c>
@@ -15250,7 +15215,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>74359</v>
       </c>
@@ -15305,7 +15270,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>45110</v>
       </c>
@@ -15363,7 +15328,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>45040</v>
       </c>
@@ -15418,7 +15383,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>46328</v>
       </c>
@@ -15473,7 +15438,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>71925</v>
       </c>
@@ -15528,7 +15493,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>45143</v>
       </c>
@@ -15583,7 +15548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>74679</v>
       </c>
@@ -15641,7 +15606,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>74373</v>
       </c>
@@ -15696,7 +15661,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>74374</v>
       </c>
@@ -15754,7 +15719,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>74683</v>
       </c>
@@ -15809,7 +15774,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>45091</v>
       </c>
@@ -15873,20 +15838,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -15932,13 +15897,13 @@
         <v>400</v>
       </c>
       <c r="F2" s="16">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="G2" s="16">
-        <v>600</v>
+        <v>3600</v>
       </c>
       <c r="H2" s="16">
-        <v>60</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -15948,17 +15913,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Final commit for  s.witkin.
Now using CO2 capacities to define capex, k , and capacity of locations.
next, will need to make final moves to eliminate Plant Size [MW] column.
</commit_message>
<xml_diff>
--- a/input_BAT2030.xlsx
+++ b/input_BAT2030.xlsx
@@ -3963,8 +3963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J40" sqref="J40:J41"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15842,7 +15842,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15900,7 +15900,7 @@
         <v>1E-3</v>
       </c>
       <c r="G2" s="16">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="H2" s="16">
         <v>-1</v>

</xml_diff>

<commit_message>
Added Fuel Produced amount to output table
</commit_message>
<xml_diff>
--- a/input_BAT2030.xlsx
+++ b/input_BAT2030.xlsx
@@ -3963,8 +3963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15842,7 +15842,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15900,7 +15900,7 @@
         <v>1E-3</v>
       </c>
       <c r="G2" s="16">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="H2" s="16">
         <v>-1</v>

</xml_diff>